<commit_message>
Pretty simple. Like my solution
</commit_message>
<xml_diff>
--- a/CH-121 Power.xlsx
+++ b/CH-121 Power.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{922B9994-344E-49B6-872C-720CFE309D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB274C5-C7C6-4795-BC6C-1E072D553944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,10 +35,35 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/omid-motamedisedeh-74aba166/recent-activity/all/</t>
   </si>
 </sst>
 </file>
@@ -101,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -244,11 +269,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -284,6 +444,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="C15" sqref="C15:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,7 +964,7 @@
     <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
@@ -804,8 +973,11 @@
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
-    </row>
-    <row r="2" spans="2:8" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -814,7 +986,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:8" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C3" s="11">
         <v>1</v>
       </c>
@@ -834,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -854,7 +1026,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C5" s="3">
         <v>3</v>
       </c>
@@ -874,7 +1046,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C6" s="3">
         <v>4</v>
       </c>
@@ -894,7 +1066,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="7" spans="2:8" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C7" s="3">
         <v>5</v>
       </c>
@@ -914,7 +1086,7 @@
         <v>15625</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C8" s="5">
         <v>6</v>
       </c>
@@ -934,7 +1106,7 @@
         <v>46656</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
@@ -942,7 +1114,7 @@
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
@@ -950,13 +1122,134 @@
       <c r="G10"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C15" s="17" cm="1">
+        <f t="array" ref="C15:H20">_xlfn.MAKEARRAY(6,6,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,_xlpm.r^_xlpm.c))</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="18">
+        <v>1</v>
+      </c>
+      <c r="E15" s="18">
+        <v>1</v>
+      </c>
+      <c r="F15" s="18">
+        <v>1</v>
+      </c>
+      <c r="G15" s="18">
+        <v>1</v>
+      </c>
+      <c r="H15" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C16" s="20">
+        <v>2</v>
+      </c>
+      <c r="D16" s="21">
+        <v>4</v>
+      </c>
+      <c r="E16" s="21">
+        <v>8</v>
+      </c>
+      <c r="F16" s="21">
+        <v>16</v>
+      </c>
+      <c r="G16" s="21">
+        <v>32</v>
+      </c>
+      <c r="H16" s="22">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="20">
+        <v>3</v>
+      </c>
+      <c r="D17" s="21">
+        <v>9</v>
+      </c>
+      <c r="E17" s="21">
+        <v>27</v>
+      </c>
+      <c r="F17" s="21">
+        <v>81</v>
+      </c>
+      <c r="G17" s="21">
+        <v>243</v>
+      </c>
+      <c r="H17" s="22">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C18" s="20">
+        <v>4</v>
+      </c>
+      <c r="D18" s="21">
+        <v>16</v>
+      </c>
+      <c r="E18" s="21">
+        <v>64</v>
+      </c>
+      <c r="F18" s="21">
+        <v>256</v>
+      </c>
+      <c r="G18" s="21">
+        <v>1024</v>
+      </c>
+      <c r="H18" s="22">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C19" s="20">
+        <v>5</v>
+      </c>
+      <c r="D19" s="21">
+        <v>25</v>
+      </c>
+      <c r="E19" s="21">
+        <v>125</v>
+      </c>
+      <c r="F19" s="21">
+        <v>625</v>
+      </c>
+      <c r="G19" s="21">
+        <v>3125</v>
+      </c>
+      <c r="H19" s="22">
+        <v>15625</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C20" s="23">
+        <v>6</v>
+      </c>
+      <c r="D20" s="24">
+        <v>36</v>
+      </c>
+      <c r="E20" s="24">
+        <v>216</v>
+      </c>
+      <c r="F20" s="24">
+        <v>1296</v>
+      </c>
+      <c r="G20" s="24">
+        <v>7776</v>
+      </c>
+      <c r="H20" s="25">
+        <v>46656</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>